<commit_message>
updated the structure of the repo
</commit_message>
<xml_diff>
--- a/Testing/IMU data/joltGyro.xlsx
+++ b/Testing/IMU data/joltGyro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tris/Documents/2022UCT/2nd sem/3097/SHARC_buoy_data_transmission/Testing/IMU data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{705E6F22-4359-3E49-B1BB-7D11793E2D31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AF0AB44-9724-E643-A8F0-A703A65A9A8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{B2251EFB-11C5-9C46-9903-56D75794EB29}"/>
   </bookViews>
@@ -145,7 +145,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>Gyrometer</a:t>
+              <a:t>Gyroscope</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-GB" baseline="0"/>

</xml_diff>